<commit_message>
Petite erreur dans la détermination des features
</commit_message>
<xml_diff>
--- a/Docs/Résultats/Résultats_25_01_16.xlsx
+++ b/Docs/Résultats/Résultats_25_01_16.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Titre</t>
   </si>
@@ -177,13 +177,10 @@
     <t>48 notes de la guitare</t>
   </si>
   <si>
-    <t>Prise en compte des silences</t>
-  </si>
-  <si>
-    <t>Ajout d'un morceau</t>
-  </si>
-  <si>
-    <t>*</t>
+    <t>Changement de méthode pour le tempo</t>
+  </si>
+  <si>
+    <t>prise en compte de la dernière note</t>
   </si>
 </sst>
 </file>
@@ -707,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,8 +727,8 @@
     <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="14" t="s">
         <v>0</v>
@@ -771,7 +768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>1</v>
       </c>
@@ -816,7 +813,7 @@
         <v>0.80952400000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -855,13 +852,13 @@
         <v>0.50833333333333297</v>
       </c>
       <c r="M4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -894,19 +891,19 @@
         <v>1</v>
       </c>
       <c r="K5" s="5">
-        <v>0.97297297297297303</v>
+        <v>0.96969696969696995</v>
       </c>
       <c r="L5" s="4">
         <v>0.96666666666666701</v>
       </c>
       <c r="M5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -939,19 +936,19 @@
         <v>1</v>
       </c>
       <c r="K6" s="5">
-        <v>0.89743589743589791</v>
+        <v>0.85185185185185208</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
       </c>
       <c r="M6" s="5">
-        <v>1</v>
+        <v>0.92307692307692302</v>
       </c>
       <c r="N6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -981,7 +978,7 @@
         <v>42.913043478260889</v>
       </c>
       <c r="J7" s="9">
-        <v>0.82926829268292712</v>
+        <v>0.84615384615384603</v>
       </c>
       <c r="K7" s="5">
         <v>1</v>
@@ -990,13 +987,13 @@
         <v>0.241666666666667</v>
       </c>
       <c r="M7" s="5">
-        <v>0.34139999999999998</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="N7" s="5">
         <v>0.75609800000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1026,25 +1023,22 @@
         <v>81.900000000000006</v>
       </c>
       <c r="J8" s="9">
-        <v>0.875</v>
+        <v>0.90625</v>
       </c>
       <c r="K8" s="5">
-        <v>0.70833333333333304</v>
+        <v>0.703125</v>
       </c>
       <c r="L8" s="4">
         <v>8.0645161290322596E-3</v>
       </c>
       <c r="M8" s="5">
-        <v>0.12670000000000001</v>
+        <v>0.79166666666666696</v>
       </c>
       <c r="N8" s="5">
         <v>0.81689999999999996</v>
       </c>
-      <c r="O8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1083,13 +1077,13 @@
         <v>0.1</v>
       </c>
       <c r="M9" s="5">
-        <v>0.69699999999999995</v>
+        <v>0.87301587301587302</v>
       </c>
       <c r="N9" s="5">
         <v>0.81810000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1119,22 +1113,22 @@
         <v>82.942528735632195</v>
       </c>
       <c r="J10" s="9">
-        <v>0.88888888888888895</v>
+        <v>0.88157894736842091</v>
       </c>
       <c r="K10" s="5">
-        <v>0.97530864197530898</v>
+        <v>0.97368421052631604</v>
       </c>
       <c r="L10" s="4">
         <v>0.17708333333333301</v>
       </c>
       <c r="M10" s="5">
-        <v>0.42199999999999999</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="N10" s="5">
         <v>0.73499999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1164,22 +1158,22 @@
         <v>77.962500000000006</v>
       </c>
       <c r="J11" s="9">
-        <v>0.98666666666666702</v>
+        <v>0.984375</v>
       </c>
       <c r="K11" s="5">
-        <v>0.98666666666666702</v>
+        <v>0.984375</v>
       </c>
       <c r="L11" s="4">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="M11" s="5">
-        <v>0.84</v>
+        <v>0.83783783783783805</v>
       </c>
       <c r="N11" s="5">
         <v>0.84</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1209,22 +1203,22 @@
         <v>72.92307692307692</v>
       </c>
       <c r="J12" s="9">
-        <v>0.83333333333333304</v>
+        <v>0.81818181818181801</v>
       </c>
       <c r="K12" s="5">
-        <v>0.81818181818181801</v>
+        <v>0.78181818181818197</v>
       </c>
       <c r="L12" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M12" s="5">
-        <v>0.83819999999999995</v>
+        <v>0.83582089552238803</v>
       </c>
       <c r="N12" s="5">
         <v>0.83819999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -1254,7 +1248,7 @@
         <v>368.98395721925135</v>
       </c>
       <c r="J13" s="10">
-        <v>0.99719101123595488</v>
+        <v>0.99692307692307691</v>
       </c>
       <c r="K13" s="8">
         <v>1</v>
@@ -1269,7 +1263,7 @@
         <v>0.97799999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="26" t="s">
         <v>19</v>
       </c>
@@ -1291,11 +1285,11 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7">
         <f>SUMPRODUCT($E$4:$E$13,J4:J13)/SUM($E$4:$E$13)</f>
-        <v>0.94951413221936654</v>
+        <v>0.95114767394372668</v>
       </c>
       <c r="K14" s="7">
         <f>SUMPRODUCT(E4:E13,K4:K13)/SUM(E4:E13)</f>
-        <v>0.94431356120184962</v>
+        <v>0.93823452280031239</v>
       </c>
       <c r="L14" s="7">
         <f>SUMPRODUCT(E3:E13,L3:L13)/SUM(E3:E13)</f>
@@ -1303,14 +1297,14 @@
       </c>
       <c r="M14" s="7">
         <f>SUMPRODUCT(E3:E13,M3:M13)/SUM(E3:E13)</f>
-        <v>0.76269376321353066</v>
+        <v>0.78773210392387771</v>
       </c>
       <c r="N14" s="8">
         <f>SUMPRODUCT(E3:E13,N3:N13)/SUM(E3:E13)</f>
         <v>0.89199715644820288</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
         <v>27</v>
       </c>
@@ -1343,7 +1337,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>28</v>
       </c>
@@ -1357,11 +1351,11 @@
       </c>
       <c r="J16" s="25">
         <f>J14-[1]Feuil1!J$14</f>
-        <v>0</v>
+        <v>1.6335417243601436E-3</v>
       </c>
       <c r="K16" s="25">
         <f>K14-[1]Feuil1!K$14</f>
-        <v>0</v>
+        <v>-6.079038401537229E-3</v>
       </c>
       <c r="L16" s="25">
         <f>L14-[1]Feuil1!L$14</f>
@@ -1369,7 +1363,7 @@
       </c>
       <c r="M16" s="25">
         <f>M14-[1]Feuil1!M$14</f>
-        <v>0</v>
+        <v>2.5038340710347051E-2</v>
       </c>
       <c r="N16" s="25">
         <f>N14-[1]Feuil1!N$14</f>
@@ -1383,92 +1377,250 @@
       <c r="C18" s="18" t="s">
         <v>20</v>
       </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f>P18/100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="3:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>30</v>
       </c>
+      <c r="K19">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="L19">
+        <v>72.2222222222222</v>
+      </c>
+      <c r="M19">
+        <f>K19/100</f>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="N19">
+        <f>L19/100</f>
+        <v>0.72222222222222199</v>
+      </c>
       <c r="P19">
-        <v>50.8333333333333</v>
-      </c>
-      <c r="Q19" s="4">
-        <f>ABS(P19/100)</f>
-        <v>0.50833333333333297</v>
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" ref="Q19:Q26" si="1">P19/100</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>31</v>
       </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <v>100</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ref="M20:M29" si="2">K20/100</f>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ref="N20:N29" si="3">L20/100</f>
+        <v>1</v>
+      </c>
       <c r="P20">
-        <v>-96.6666666666667</v>
-      </c>
-      <c r="Q20" s="4">
-        <f t="shared" ref="Q20:Q27" si="1">ABS(P20/100)</f>
-        <v>0.96666666666666701</v>
+        <v>92.307692307692307</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="1"/>
+        <v>0.92307692307692302</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>96.969696969696997</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>0.96969696969696995</v>
+      </c>
       <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="Q21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>85.185185185185205</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="3"/>
+        <v>0.85185185185185208</v>
+      </c>
       <c r="P22">
-        <v>24.1666666666667</v>
-      </c>
-      <c r="Q22" s="4">
+        <v>79.1666666666667</v>
+      </c>
+      <c r="Q22">
         <f t="shared" si="1"/>
-        <v>0.241666666666667</v>
+        <v>0.79166666666666696</v>
       </c>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>84.615384615384599</v>
+      </c>
+      <c r="L23">
+        <v>100</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="2"/>
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="P23">
-        <v>0.80645161290322598</v>
-      </c>
-      <c r="Q23" s="4">
+        <v>87.301587301587304</v>
+      </c>
+      <c r="Q23">
         <f t="shared" si="1"/>
-        <v>8.0645161290322596E-3</v>
+        <v>0.87301587301587302</v>
       </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>90.625</v>
+      </c>
+      <c r="L24">
+        <v>70.3125</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>0.90625</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="3"/>
+        <v>0.703125</v>
+      </c>
       <c r="P24">
-        <v>-10</v>
-      </c>
-      <c r="Q24" s="4">
+        <v>52.5</v>
+      </c>
+      <c r="Q24">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>96.825396825396794</v>
+      </c>
+      <c r="L25">
+        <v>96.825396825396794</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="2"/>
+        <v>0.96825396825396792</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>0.96825396825396792</v>
+      </c>
       <c r="P25">
-        <v>-17.7083333333333</v>
-      </c>
-      <c r="Q25" s="4">
+        <v>83.783783783783804</v>
+      </c>
+      <c r="Q25">
         <f t="shared" si="1"/>
-        <v>0.17708333333333301</v>
+        <v>0.83783783783783805</v>
       </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>88.157894736842096</v>
+      </c>
+      <c r="L26">
+        <v>97.368421052631604</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="2"/>
+        <v>0.88157894736842091</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="3"/>
+        <v>0.97368421052631604</v>
+      </c>
       <c r="P26">
-        <v>-1.25</v>
-      </c>
-      <c r="Q26" s="4">
+        <v>83.582089552238799</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="1"/>
-        <v>1.2500000000000001E-2</v>
+        <v>0.83582089552238803</v>
       </c>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="P27">
-        <v>-2.5</v>
-      </c>
-      <c r="Q27" s="4">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
+      <c r="K27">
+        <v>98.4375</v>
+      </c>
+      <c r="L27">
+        <v>98.4375</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="2"/>
+        <v>0.984375</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>0.984375</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>81.818181818181799</v>
+      </c>
+      <c r="L28">
+        <v>78.181818181818201</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>0.81818181818181801</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="3"/>
+        <v>0.78181818181818197</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>99.692307692307693</v>
+      </c>
+      <c r="L29">
+        <v>100</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>0.99692307692307691</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1652,18 +1804,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q19:Q27">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.25"/>
-        <cfvo type="num" val="0.5"/>
-        <color rgb="FF92D050"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>